<commit_message>
Fleshing out project import and unit tests
</commit_message>
<xml_diff>
--- a/tests/Homesite.Infrastructure.Tests/Assets/ProjectImportTestAsset.xlsx
+++ b/tests/Homesite.Infrastructure.Tests/Assets/ProjectImportTestAsset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\OldKayakFisherman\Homesite\tests\Homesite.Infrastructure.Tests\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6AF10C-F9ED-4ADF-809C-534D64977DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BE48E0-5552-48CF-93EB-95DEE618F9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFC65C7A-5930-4928-86AB-91C1F7697366}"/>
   </bookViews>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A12CCB-AE1B-49B3-888E-D01A9C55737A}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>